<commit_message>
Actualizando el flujo de datos y resultado
</commit_message>
<xml_diff>
--- a/ConsolidadoFacturacionPais.xlsx
+++ b/ConsolidadoFacturacionPais.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29127"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luis Mart\Downloads\Datawarehouse y Minería de Datos DMD941 G01T\DesafioPractico1_CM170741\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A4D90C1-F282-44AD-AFA9-8AC1FD00CBC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,9 +24,23 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+  <si>
+    <t>Total de Ventas</t>
+  </si>
+  <si>
+    <t>Monto de Facturación</t>
+  </si>
+  <si>
+    <t>Nombre País</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -28,13 +48,26 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -49,8 +82,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -330,13 +366,32 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="18.5546875" customWidth="1"/>
+    <col min="2" max="2" width="21.21875" customWidth="1"/>
+    <col min="3" max="3" width="24.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Publicacion de los cambios con los resultados
</commit_message>
<xml_diff>
--- a/ConsolidadoFacturacionPais.xlsx
+++ b/ConsolidadoFacturacionPais.xlsx
@@ -366,10 +366,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0" rightToLeft="false">
       <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
@@ -380,7 +380,7 @@
     <col min="3" max="3" width="24.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row spans="1:3" ht="19.2" customHeight="1" x14ac:dyDescent="0.3" outlineLevel="0" r="1">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -389,6 +389,57 @@
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2">
+      <c r="A2" s="0" t="inlineStr">
+        <is>
+          <t>Honduras</t>
+        </is>
+      </c>
+      <c r="B2" s="0" t="inlineStr">
+        <is>
+          <t>80</t>
+        </is>
+      </c>
+      <c r="C2" s="0" t="inlineStr">
+        <is>
+          <t>8703.10</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="3">
+      <c r="A3" s="0" t="inlineStr">
+        <is>
+          <t>Guatemala</t>
+        </is>
+      </c>
+      <c r="B3" s="0" t="inlineStr">
+        <is>
+          <t>80</t>
+        </is>
+      </c>
+      <c r="C3" s="0" t="inlineStr">
+        <is>
+          <t>8344.90</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="4">
+      <c r="A4" s="0" t="inlineStr">
+        <is>
+          <t>Costa Rica</t>
+        </is>
+      </c>
+      <c r="B4" s="0" t="inlineStr">
+        <is>
+          <t>80</t>
+        </is>
+      </c>
+      <c r="C4" s="0" t="inlineStr">
+        <is>
+          <t>9503.10</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>